<commit_message>
Add additional activities to Gantt chart
</commit_message>
<xml_diff>
--- a/TempestTraceGanttChart.xlsx
+++ b/TempestTraceGanttChart.xlsx
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Plan</t>
   </si>
@@ -117,15 +117,6 @@
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
   </si>
   <si>
     <t>Activity 14</t>
@@ -315,6 +306,18 @@
   </si>
   <si>
     <t>Aircon steam release</t>
+  </si>
+  <si>
+    <t>Two player split screen</t>
+  </si>
+  <si>
+    <t>Menus</t>
+  </si>
+  <si>
+    <t>Intro flyover deployed</t>
+  </si>
+  <si>
+    <t>Intro flyover script</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -759,6 +762,12 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -776,7 +785,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="74">
     <dxf>
       <fill>
         <patternFill>
@@ -1232,6 +1241,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1243,6 +1280,317 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
           <color theme="7"/>
         </bottom>
         <vertical/>
@@ -1256,6 +1604,119 @@
         </top>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1679,10 +2140,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:BJ41"/>
+  <dimension ref="A2:BJ42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A23" sqref="A23:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1698,7 +2159,7 @@
   <sheetData>
     <row r="2" spans="1:62" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -1714,7 +2175,7 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="I3" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1734,11 +2195,11 @@
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AC3" s="13"/>
       <c r="AD3" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
@@ -1746,7 +2207,7 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="14"/>
       <c r="AL3" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1764,19 +2225,19 @@
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="P5" s="30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q5" s="28"/>
       <c r="R5" s="26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="X5" s="27"/>
       <c r="Y5" s="26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AE5" s="29"/>
       <c r="AF5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
@@ -1825,7 +2286,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I7" s="25" t="s">
         <v>8</v>
@@ -2083,7 +2544,7 @@
     </row>
     <row r="10" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="31"/>
       <c r="C10" s="15"/>
@@ -2095,7 +2556,7 @@
     <row r="11" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
       <c r="B11" s="32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="15">
         <v>2</v>
@@ -2115,23 +2576,23 @@
       <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36">
+      <c r="A12" s="41">
         <v>1</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12" s="15">
         <v>4</v>
       </c>
       <c r="D12" s="15">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E12" s="15">
         <v>4</v>
       </c>
       <c r="F12" s="15">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G12" s="33">
         <v>0.25</v>
@@ -2139,11 +2600,11 @@
       <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36">
+      <c r="A13" s="41">
         <v>2</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13" s="15">
         <v>16</v>
@@ -2160,14 +2621,17 @@
       <c r="G13" s="33">
         <v>0</v>
       </c>
-      <c r="H13" s="34"/>
+      <c r="H13" s="42" t="str">
+        <f>CONCATENATE(A12, ", ", A26)</f>
+        <v>1, 12</v>
+      </c>
     </row>
     <row r="14" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36">
+      <c r="A14" s="41">
         <v>3</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14" s="15">
         <v>29</v>
@@ -2191,7 +2655,7 @@
     </row>
     <row r="15" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B15" s="39"/>
       <c r="C15" s="15"/>
@@ -2201,11 +2665,11 @@
       <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36">
+      <c r="A16" s="41">
         <v>4</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="15">
         <v>6</v>
@@ -2225,11 +2689,11 @@
       <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36">
+      <c r="A17" s="41">
         <v>5</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" s="15">
         <v>17</v>
@@ -2249,39 +2713,39 @@
       <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="41">
+        <v>6</v>
+      </c>
+      <c r="B18" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="33"/>
+      <c r="C18" s="15">
+        <v>22</v>
+      </c>
+      <c r="D18" s="15">
+        <v>4</v>
+      </c>
+      <c r="E18" s="15">
+        <v>22</v>
+      </c>
+      <c r="F18" s="15">
+        <v>4</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0</v>
+      </c>
       <c r="H18" s="34"/>
     </row>
     <row r="19" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36">
-        <v>6</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="15">
-        <v>22</v>
-      </c>
-      <c r="D19" s="15">
-        <v>7</v>
-      </c>
-      <c r="E19" s="15">
-        <v>22</v>
-      </c>
-      <c r="F19" s="15">
-        <v>7</v>
-      </c>
-      <c r="G19" s="33">
-        <v>0</v>
-      </c>
+      <c r="A19" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="33"/>
       <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2289,106 +2753,106 @@
         <v>7</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C20" s="15">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D20" s="15">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E20" s="15">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F20" s="15">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G20" s="33">
         <v>0</v>
       </c>
-      <c r="H20" s="34">
-        <f>A19</f>
-        <v>6</v>
-      </c>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36">
         <v>8</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C21" s="15">
         <v>29</v>
       </c>
       <c r="D21" s="15">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E21" s="15">
         <v>29</v>
       </c>
       <c r="F21" s="15">
+        <v>14</v>
+      </c>
+      <c r="G21" s="33">
+        <v>0</v>
+      </c>
+      <c r="H21" s="34">
+        <f>A20</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="36">
         <v>9</v>
       </c>
-      <c r="G21" s="33">
-        <v>0</v>
-      </c>
-      <c r="H21" s="34">
-        <f>A19</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="34"/>
+      <c r="B22" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="15">
+        <v>29</v>
+      </c>
+      <c r="D22" s="15">
+        <v>9</v>
+      </c>
+      <c r="E22" s="15">
+        <v>29</v>
+      </c>
+      <c r="F22" s="15">
+        <v>9</v>
+      </c>
+      <c r="G22" s="33">
+        <v>0</v>
+      </c>
+      <c r="H22" s="34">
+        <f>A20</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="36">
-        <v>9</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="15">
-        <v>37</v>
-      </c>
-      <c r="D23" s="15">
-        <v>5</v>
-      </c>
-      <c r="E23" s="15">
-        <v>37</v>
-      </c>
-      <c r="F23" s="15">
-        <v>5</v>
-      </c>
-      <c r="G23" s="33">
-        <v>0</v>
-      </c>
+      <c r="A23" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="39"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="33"/>
       <c r="H23" s="34"/>
     </row>
     <row r="24" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36">
         <v>10</v>
       </c>
-      <c r="B24" s="35" t="s">
-        <v>43</v>
+      <c r="B24" s="40" t="s">
+        <v>35</v>
       </c>
       <c r="C24" s="15">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D24" s="15">
         <v>5</v>
       </c>
       <c r="E24" s="15">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F24" s="15">
         <v>5</v>
@@ -2400,19 +2864,19 @@
     </row>
     <row r="25" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="36">
-        <v>12</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>51</v>
+        <v>11</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>40</v>
       </c>
       <c r="C25" s="15">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D25" s="15">
         <v>5</v>
       </c>
       <c r="E25" s="15">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="F25" s="15">
         <v>5</v>
@@ -2424,22 +2888,22 @@
     </row>
     <row r="26" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="36">
-        <v>13</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="17">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="15">
+        <v>9</v>
       </c>
       <c r="D26" s="15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E26" s="15">
+        <v>9</v>
+      </c>
+      <c r="F26" s="15">
         <v>5</v>
-      </c>
-      <c r="F26" s="15">
-        <v>8</v>
       </c>
       <c r="G26" s="33">
         <v>0</v>
@@ -2448,19 +2912,19 @@
     </row>
     <row r="27" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="36">
-        <v>14</v>
-      </c>
-      <c r="B27" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="15">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="17">
+        <v>16</v>
       </c>
       <c r="D27" s="15">
         <v>3</v>
       </c>
       <c r="E27" s="15">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F27" s="15">
         <v>3</v>
@@ -2468,50 +2932,53 @@
       <c r="G27" s="33">
         <v>0</v>
       </c>
-      <c r="H27" s="34"/>
+      <c r="H27" s="42">
+        <f>A12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="36">
-        <v>15</v>
-      </c>
-      <c r="B28" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="15">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="17">
+        <v>2</v>
       </c>
       <c r="D28" s="15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E28" s="15">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F28" s="15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G28" s="33">
-        <v>0</v>
-      </c>
-      <c r="H28" s="34"/>
+        <v>1</v>
+      </c>
+      <c r="H28" s="42"/>
     </row>
     <row r="29" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="36">
-        <v>16</v>
-      </c>
-      <c r="B29" s="38" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>50</v>
       </c>
       <c r="C29" s="15">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D29" s="15">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E29" s="15">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="F29" s="15">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G29" s="33">
         <v>0</v>
@@ -2520,22 +2987,22 @@
     </row>
     <row r="30" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="36">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C30" s="15">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D30" s="15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E30" s="15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F30" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G30" s="33">
         <v>0</v>
@@ -2544,22 +3011,22 @@
     </row>
     <row r="31" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="36">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C31" s="15">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D31" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E31" s="15">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F31" s="15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G31" s="33">
         <v>0</v>
@@ -2568,22 +3035,22 @@
     </row>
     <row r="32" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="36">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C32" s="15">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D32" s="15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E32" s="15">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F32" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G32" s="33">
         <v>0</v>
@@ -2592,22 +3059,22 @@
     </row>
     <row r="33" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="36">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C33" s="15">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D33" s="15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E33" s="15">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F33" s="15">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G33" s="33">
         <v>0</v>
@@ -2616,22 +3083,22 @@
     </row>
     <row r="34" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="36">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C34" s="15">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D34" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" s="15">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F34" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G34" s="33">
         <v>0</v>
@@ -2640,22 +3107,22 @@
     </row>
     <row r="35" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="36">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C35" s="15">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D35" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E35" s="15">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F35" s="15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G35" s="33">
         <v>0</v>
@@ -2664,22 +3131,22 @@
     </row>
     <row r="36" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="36">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C36" s="15">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D36" s="15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E36" s="15">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F36" s="15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G36" s="33">
         <v>0</v>
@@ -2688,22 +3155,22 @@
     </row>
     <row r="37" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="36">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C37" s="15">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D37" s="15">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E37" s="15">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F37" s="15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G37" s="33">
         <v>0</v>
@@ -2712,22 +3179,22 @@
     </row>
     <row r="38" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="36">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C38" s="15">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D38" s="15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E38" s="15">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F38" s="15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G38" s="33">
         <v>0</v>
@@ -2736,46 +3203,46 @@
     </row>
     <row r="39" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="36">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C39" s="15">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D39" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E39" s="15">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F39" s="15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G39" s="33">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H39" s="34"/>
     </row>
     <row r="40" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="36">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C40" s="15">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D40" s="15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E40" s="15">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F40" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G40" s="33">
         <v>0</v>
@@ -2784,32 +3251,56 @@
     </row>
     <row r="41" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="36">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B41" s="38" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C41" s="15">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D41" s="15">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="E41" s="15">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F41" s="15">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G41" s="33">
         <v>0</v>
       </c>
       <c r="H41" s="34"/>
+    </row>
+    <row r="42" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="36">
+        <v>27</v>
+      </c>
+      <c r="B42" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="15">
+        <v>0</v>
+      </c>
+      <c r="D42" s="15">
+        <v>0</v>
+      </c>
+      <c r="E42" s="15">
+        <v>0</v>
+      </c>
+      <c r="F42" s="15">
+        <v>0</v>
+      </c>
+      <c r="G42" s="33">
+        <v>0</v>
+      </c>
+      <c r="H42" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="BF8:BI8"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="A10:B10"/>
@@ -2823,143 +3314,195 @@
     <mergeCell ref="P8:V8"/>
     <mergeCell ref="W8:AC8"/>
   </mergeCells>
-  <conditionalFormatting sqref="I11:BI14 I16:BI17 I19:BI21 I23:BI41">
-    <cfRule type="expression" dxfId="41" priority="33">
+  <conditionalFormatting sqref="I11:BI14 I16:BI16 I20:BI22 I24:BI26 I18:BI18 I28:BI42">
+    <cfRule type="expression" dxfId="65" priority="49">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="35">
+    <cfRule type="expression" dxfId="64" priority="51">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="36">
+    <cfRule type="expression" dxfId="63" priority="52">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="37">
+    <cfRule type="expression" dxfId="62" priority="53">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="38">
+    <cfRule type="expression" dxfId="61" priority="54">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="39">
+    <cfRule type="expression" dxfId="60" priority="55">
       <formula>I$9=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="43">
+    <cfRule type="expression" dxfId="59" priority="59">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="44">
+    <cfRule type="expression" dxfId="58" priority="60">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42:BJ42">
-    <cfRule type="expression" dxfId="33" priority="34">
+  <conditionalFormatting sqref="B43:BJ43">
+    <cfRule type="expression" dxfId="57" priority="50">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:BI9">
-    <cfRule type="expression" dxfId="32" priority="40">
+    <cfRule type="expression" dxfId="56" priority="56">
       <formula>I$9=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BI10">
-    <cfRule type="expression" dxfId="31" priority="25">
+    <cfRule type="expression" dxfId="55" priority="41">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26">
+    <cfRule type="expression" dxfId="54" priority="42">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="27">
+    <cfRule type="expression" dxfId="53" priority="43">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28">
+    <cfRule type="expression" dxfId="52" priority="44">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="29">
+    <cfRule type="expression" dxfId="51" priority="45">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="30">
+    <cfRule type="expression" dxfId="50" priority="46">
       <formula>I$9=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="31">
+    <cfRule type="expression" dxfId="49" priority="47">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="32">
+    <cfRule type="expression" dxfId="48" priority="48">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:BI15">
-    <cfRule type="expression" dxfId="23" priority="17">
+    <cfRule type="expression" dxfId="47" priority="33">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18">
+    <cfRule type="expression" dxfId="46" priority="34">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="19">
+    <cfRule type="expression" dxfId="45" priority="35">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="20">
+    <cfRule type="expression" dxfId="44" priority="36">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21">
+    <cfRule type="expression" dxfId="43" priority="37">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="42" priority="38">
       <formula>I$9=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="23">
+    <cfRule type="expression" dxfId="41" priority="39">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="24">
+    <cfRule type="expression" dxfId="40" priority="40">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:BI18">
-    <cfRule type="expression" dxfId="15" priority="9">
+  <conditionalFormatting sqref="I19:BI19">
+    <cfRule type="expression" dxfId="39" priority="25">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="38" priority="26">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="37" priority="27">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="36" priority="28">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="35" priority="29">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="34" priority="30">
       <formula>I$9=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
+    <cfRule type="expression" dxfId="33" priority="31">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16">
+    <cfRule type="expression" dxfId="32" priority="32">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22:BI22">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="I23:BI23">
+    <cfRule type="expression" dxfId="31" priority="17">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="30" priority="18">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="29" priority="19">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="28" priority="20">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="27" priority="21">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="26" priority="22">
       <formula>I$9=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="25" priority="23">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="24" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17:BI17">
+    <cfRule type="expression" dxfId="23" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="14">
+      <formula>I$9=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27:BI27">
+    <cfRule type="expression" dxfId="15" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>I$9=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add level geometry exporter to gantt chart
</commit_message>
<xml_diff>
--- a/TempestTraceGanttChart.xlsx
+++ b/TempestTraceGanttChart.xlsx
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Plan</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>Smoke bomb</t>
+  </si>
+  <si>
+    <t>Level geometry exporter</t>
   </si>
 </sst>
 </file>
@@ -751,6 +754,15 @@
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="12" borderId="0" xfId="12" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="11" borderId="0" xfId="11" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -765,15 +777,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="11" borderId="0" xfId="11" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="12" borderId="0" xfId="12" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -791,7 +794,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="106">
     <dxf>
       <fill>
         <patternFill>
@@ -1812,6 +1815,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1823,6 +1854,91 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
           <color theme="7"/>
         </bottom>
         <vertical/>
@@ -1836,6 +1952,119 @@
         </top>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2372,10 +2601,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:BJ44"/>
+  <dimension ref="A2:BJ45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2390,22 +2619,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:62" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:62" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
       <c r="I3" s="8" t="s">
         <v>24</v>
       </c>
@@ -2443,12 +2672,12 @@
       </c>
     </row>
     <row r="4" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
@@ -2520,11 +2749,11 @@
       <c r="H7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="I7" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
     </row>
     <row r="8" spans="1:62" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
@@ -2534,75 +2763,75 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="41">
+      <c r="I8" s="36">
         <v>42218</v>
       </c>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="40">
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="37">
         <v>42225</v>
       </c>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="40"/>
-      <c r="T8" s="40"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="40"/>
-      <c r="W8" s="41">
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="37"/>
+      <c r="W8" s="36">
         <v>42232</v>
       </c>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
-      <c r="AB8" s="41"/>
-      <c r="AC8" s="41"/>
-      <c r="AD8" s="40">
+      <c r="X8" s="36"/>
+      <c r="Y8" s="36"/>
+      <c r="Z8" s="36"/>
+      <c r="AA8" s="36"/>
+      <c r="AB8" s="36"/>
+      <c r="AC8" s="36"/>
+      <c r="AD8" s="37">
         <v>42239</v>
       </c>
-      <c r="AE8" s="40"/>
-      <c r="AF8" s="40"/>
-      <c r="AG8" s="40"/>
-      <c r="AH8" s="40"/>
-      <c r="AI8" s="40"/>
-      <c r="AJ8" s="40"/>
-      <c r="AK8" s="41">
+      <c r="AE8" s="37"/>
+      <c r="AF8" s="37"/>
+      <c r="AG8" s="37"/>
+      <c r="AH8" s="37"/>
+      <c r="AI8" s="37"/>
+      <c r="AJ8" s="37"/>
+      <c r="AK8" s="36">
         <v>42246</v>
       </c>
-      <c r="AL8" s="41"/>
-      <c r="AM8" s="41"/>
-      <c r="AN8" s="41"/>
-      <c r="AO8" s="41"/>
-      <c r="AP8" s="41"/>
-      <c r="AQ8" s="41"/>
-      <c r="AR8" s="40">
+      <c r="AL8" s="36"/>
+      <c r="AM8" s="36"/>
+      <c r="AN8" s="36"/>
+      <c r="AO8" s="36"/>
+      <c r="AP8" s="36"/>
+      <c r="AQ8" s="36"/>
+      <c r="AR8" s="37">
         <v>42253</v>
       </c>
-      <c r="AS8" s="40"/>
-      <c r="AT8" s="40"/>
-      <c r="AU8" s="40"/>
-      <c r="AV8" s="40"/>
-      <c r="AW8" s="40"/>
-      <c r="AX8" s="40"/>
-      <c r="AY8" s="41">
+      <c r="AS8" s="37"/>
+      <c r="AT8" s="37"/>
+      <c r="AU8" s="37"/>
+      <c r="AV8" s="37"/>
+      <c r="AW8" s="37"/>
+      <c r="AX8" s="37"/>
+      <c r="AY8" s="36">
         <v>42260</v>
       </c>
-      <c r="AZ8" s="41"/>
-      <c r="BA8" s="41"/>
-      <c r="BB8" s="41"/>
-      <c r="BC8" s="41"/>
-      <c r="BD8" s="41"/>
-      <c r="BE8" s="41"/>
-      <c r="BF8" s="36">
+      <c r="AZ8" s="36"/>
+      <c r="BA8" s="36"/>
+      <c r="BB8" s="36"/>
+      <c r="BC8" s="36"/>
+      <c r="BD8" s="36"/>
+      <c r="BE8" s="36"/>
+      <c r="BF8" s="39">
         <v>42267</v>
       </c>
-      <c r="BG8" s="37"/>
-      <c r="BH8" s="37"/>
-      <c r="BI8" s="37"/>
+      <c r="BG8" s="40"/>
+      <c r="BH8" s="40"/>
+      <c r="BI8" s="40"/>
     </row>
     <row r="9" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -2775,10 +3004,10 @@
       <c r="BJ9" s="1"/>
     </row>
     <row r="10" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="39"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -2786,7 +3015,9 @@
       <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="29">
+        <v>1</v>
+      </c>
       <c r="B11" s="25" t="s">
         <v>34</v>
       </c>
@@ -2809,7 +3040,7 @@
     </row>
     <row r="12" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>39</v>
@@ -2818,13 +3049,13 @@
         <v>4</v>
       </c>
       <c r="D12" s="15">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E12" s="15">
         <v>4</v>
       </c>
       <c r="F12" s="15">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G12" s="26">
         <v>0.25</v>
@@ -2833,135 +3064,138 @@
     </row>
     <row r="13" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
-        <v>2</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>40</v>
+        <v>3</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>55</v>
       </c>
       <c r="C13" s="15">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="15">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E13" s="15">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F13" s="15">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="G13" s="26">
         <v>0</v>
       </c>
-      <c r="H13" s="34" t="str">
-        <f>CONCATENATE(A12, ", ", A28)</f>
-        <v>1, 12</v>
+      <c r="H13" s="27" t="str">
+        <f>CONCATENATE(A9)</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="15">
+        <v>17</v>
+      </c>
+      <c r="D14" s="15">
+        <v>13</v>
+      </c>
+      <c r="E14" s="15">
+        <v>17</v>
+      </c>
+      <c r="F14" s="15">
+        <v>13</v>
+      </c>
+      <c r="G14" s="26">
+        <v>0</v>
+      </c>
+      <c r="H14" s="34" t="str">
+        <f>CONCATENATE(A12, ", ", A29,", ",A13)</f>
+        <v>2, 16, 3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29">
+        <v>5</v>
+      </c>
+      <c r="B15" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="15">
-        <v>29</v>
-      </c>
-      <c r="D14" s="15">
+      <c r="C15" s="15">
+        <v>30</v>
+      </c>
+      <c r="D15" s="15">
         <v>14</v>
       </c>
-      <c r="E14" s="15">
-        <v>29</v>
-      </c>
-      <c r="F14" s="15">
+      <c r="E15" s="15">
+        <v>30</v>
+      </c>
+      <c r="F15" s="15">
         <v>14</v>
       </c>
-      <c r="G14" s="26">
-        <v>0</v>
-      </c>
-      <c r="H14" s="27" t="str">
-        <f>CONCATENATE(A12,", ", A13)</f>
-        <v>1, 2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="G15" s="26">
+        <v>0</v>
+      </c>
+      <c r="H15" s="27" t="str">
+        <f>CONCATENATE(A12,", ", A14)</f>
+        <v>2, 4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33">
-        <v>4</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="15">
-        <v>6</v>
-      </c>
-      <c r="D16" s="15">
-        <v>11</v>
-      </c>
-      <c r="E16" s="15">
-        <v>6</v>
-      </c>
-      <c r="F16" s="15">
-        <v>11</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0.05</v>
-      </c>
-      <c r="H16" s="27"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
     </row>
     <row r="17" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C17" s="15">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D17" s="15">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E17" s="15">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F17" s="15">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G17" s="26">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H17" s="27"/>
     </row>
     <row r="18" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C18" s="15">
         <v>17</v>
       </c>
       <c r="D18" s="15">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E18" s="15">
         <v>17</v>
       </c>
       <c r="F18" s="15">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G18" s="26">
         <v>0</v>
@@ -2970,22 +3204,22 @@
     </row>
     <row r="19" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C19" s="15">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D19" s="15">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E19" s="15">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F19" s="15">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G19" s="26">
         <v>0</v>
@@ -2994,169 +3228,169 @@
     </row>
     <row r="20" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33">
-        <v>6</v>
-      </c>
-      <c r="B20" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="15">
+        <v>22</v>
+      </c>
+      <c r="D20" s="15">
+        <v>4</v>
+      </c>
+      <c r="E20" s="15">
+        <v>22</v>
+      </c>
+      <c r="F20" s="15">
+        <v>4</v>
+      </c>
+      <c r="G20" s="26">
+        <v>0</v>
+      </c>
+      <c r="H20" s="27"/>
+    </row>
+    <row r="21" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="33">
+        <v>10</v>
+      </c>
+      <c r="B21" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C21" s="15">
         <v>19</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D21" s="15">
         <v>7</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E21" s="15">
         <v>19</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F21" s="15">
         <v>7</v>
       </c>
-      <c r="G20" s="26">
-        <v>0</v>
-      </c>
-      <c r="H20" s="27"/>
-    </row>
-    <row r="21" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="G21" s="26">
+        <v>0</v>
+      </c>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="27"/>
-    </row>
-    <row r="22" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
-        <v>7</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="15">
-        <v>22</v>
-      </c>
-      <c r="D22" s="15">
-        <v>7</v>
-      </c>
-      <c r="E22" s="15">
-        <v>22</v>
-      </c>
-      <c r="F22" s="15">
-        <v>7</v>
-      </c>
-      <c r="G22" s="26">
-        <v>0</v>
-      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="26"/>
       <c r="H22" s="27"/>
     </row>
     <row r="23" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
-        <v>8</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>37</v>
       </c>
       <c r="C23" s="15">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D23" s="15">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E23" s="15">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F23" s="15">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G23" s="26">
         <v>0</v>
       </c>
-      <c r="H23" s="27">
-        <f>A22</f>
-        <v>7</v>
-      </c>
+      <c r="H23" s="27"/>
     </row>
     <row r="24" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
-        <v>9</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>32</v>
+        <v>12</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="C24" s="15">
         <v>29</v>
       </c>
       <c r="D24" s="15">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E24" s="15">
         <v>29</v>
       </c>
       <c r="F24" s="15">
+        <v>14</v>
+      </c>
+      <c r="G24" s="26">
+        <v>0</v>
+      </c>
+      <c r="H24" s="27">
+        <f>A23</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
+        <v>13</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="15">
+        <v>29</v>
+      </c>
+      <c r="D25" s="15">
         <v>9</v>
       </c>
-      <c r="G24" s="26">
-        <v>0</v>
-      </c>
-      <c r="H24" s="27">
-        <f>A22</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="E25" s="15">
+        <v>29</v>
+      </c>
+      <c r="F25" s="15">
+        <v>9</v>
+      </c>
+      <c r="G25" s="26">
+        <v>0</v>
+      </c>
+      <c r="H25" s="27">
+        <f>A23</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="27"/>
-    </row>
-    <row r="26" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
-        <v>10</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="15">
-        <v>37</v>
-      </c>
-      <c r="D26" s="15">
-        <v>5</v>
-      </c>
-      <c r="E26" s="15">
-        <v>37</v>
-      </c>
-      <c r="F26" s="15">
-        <v>5</v>
-      </c>
-      <c r="G26" s="26">
-        <v>0</v>
-      </c>
+      <c r="B26" s="38"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="26"/>
       <c r="H26" s="27"/>
     </row>
     <row r="27" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
-        <v>11</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>38</v>
+        <v>14</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>33</v>
       </c>
       <c r="C27" s="15">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D27" s="15">
         <v>5</v>
       </c>
       <c r="E27" s="15">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F27" s="15">
         <v>5</v>
@@ -3168,19 +3402,19 @@
     </row>
     <row r="28" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
-        <v>12</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>46</v>
+        <v>15</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="C28" s="15">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D28" s="15">
         <v>5</v>
       </c>
       <c r="E28" s="15">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="F28" s="15">
         <v>5</v>
@@ -3192,97 +3426,97 @@
     </row>
     <row r="29" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="17">
-        <v>16</v>
+        <v>46</v>
+      </c>
+      <c r="C29" s="15">
+        <v>9</v>
       </c>
       <c r="D29" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E29" s="15">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F29" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G29" s="26">
         <v>0</v>
       </c>
-      <c r="H29" s="34">
-        <f>A12</f>
-        <v>1</v>
-      </c>
+      <c r="H29" s="27"/>
     </row>
     <row r="30" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="17">
+        <v>16</v>
+      </c>
+      <c r="D30" s="15">
+        <v>3</v>
+      </c>
+      <c r="E30" s="15">
+        <v>16</v>
+      </c>
+      <c r="F30" s="15">
+        <v>3</v>
+      </c>
+      <c r="G30" s="26">
+        <v>0</v>
+      </c>
+      <c r="H30" s="34">
+        <f>A12</f>
         <v>2</v>
       </c>
-      <c r="D30" s="15">
-        <v>2</v>
-      </c>
-      <c r="E30" s="15">
-        <v>2</v>
-      </c>
-      <c r="F30" s="15">
-        <v>2</v>
-      </c>
-      <c r="G30" s="26">
-        <v>1</v>
-      </c>
-      <c r="H30" s="34"/>
     </row>
     <row r="31" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
-        <v>14</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="15">
-        <v>40</v>
+        <v>18</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="17">
+        <v>2</v>
       </c>
       <c r="D31" s="15">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E31" s="15">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="F31" s="15">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G31" s="26">
-        <v>0</v>
-      </c>
-      <c r="H31" s="27"/>
+        <v>1</v>
+      </c>
+      <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
-        <v>15</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>51</v>
+        <v>19</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>48</v>
       </c>
       <c r="C32" s="15">
         <v>40</v>
       </c>
       <c r="D32" s="15">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E32" s="15">
         <v>40</v>
       </c>
       <c r="F32" s="15">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G32" s="26">
         <v>0</v>
@@ -3291,22 +3525,22 @@
     </row>
     <row r="33" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
-        <v>16</v>
-      </c>
-      <c r="B33" s="32" t="s">
-        <v>52</v>
+        <v>20</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>51</v>
       </c>
       <c r="C33" s="15">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D33" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E33" s="15">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F33" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G33" s="26">
         <v>0</v>
@@ -3315,22 +3549,22 @@
     </row>
     <row r="34" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29">
-        <v>17</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>52</v>
       </c>
       <c r="C34" s="15">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D34" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E34" s="15">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F34" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G34" s="26">
         <v>0</v>
@@ -3339,10 +3573,10 @@
     </row>
     <row r="35" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C35" s="15">
         <v>0</v>
@@ -3363,10 +3597,10 @@
     </row>
     <row r="36" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C36" s="15">
         <v>0</v>
@@ -3387,10 +3621,10 @@
     </row>
     <row r="37" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C37" s="15">
         <v>0</v>
@@ -3411,10 +3645,10 @@
     </row>
     <row r="38" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C38" s="15">
         <v>0</v>
@@ -3435,10 +3669,10 @@
     </row>
     <row r="39" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C39" s="15">
         <v>0</v>
@@ -3459,10 +3693,10 @@
     </row>
     <row r="40" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="15">
         <v>0</v>
@@ -3483,10 +3717,10 @@
     </row>
     <row r="41" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C41" s="15">
         <v>0</v>
@@ -3507,10 +3741,10 @@
     </row>
     <row r="42" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C42" s="15">
         <v>0</v>
@@ -3531,10 +3765,10 @@
     </row>
     <row r="43" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C43" s="15">
         <v>0</v>
@@ -3555,286 +3789,362 @@
     </row>
     <row r="44" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29">
+        <v>26</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="15">
+        <v>0</v>
+      </c>
+      <c r="D44" s="15">
+        <v>0</v>
+      </c>
+      <c r="E44" s="15">
+        <v>0</v>
+      </c>
+      <c r="F44" s="15">
+        <v>0</v>
+      </c>
+      <c r="G44" s="26">
+        <v>0</v>
+      </c>
+      <c r="H44" s="27"/>
+    </row>
+    <row r="45" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="29">
         <v>27</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B45" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="15">
-        <v>0</v>
-      </c>
-      <c r="D44" s="15">
-        <v>0</v>
-      </c>
-      <c r="E44" s="15">
-        <v>0</v>
-      </c>
-      <c r="F44" s="15">
-        <v>0</v>
-      </c>
-      <c r="G44" s="26">
-        <v>0</v>
-      </c>
-      <c r="H44" s="27"/>
+      <c r="C45" s="15">
+        <v>0</v>
+      </c>
+      <c r="D45" s="15">
+        <v>0</v>
+      </c>
+      <c r="E45" s="15">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15">
+        <v>0</v>
+      </c>
+      <c r="G45" s="26">
+        <v>0</v>
+      </c>
+      <c r="H45" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="BF8:BI8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="AD8:AJ8"/>
+    <mergeCell ref="AK8:AQ8"/>
+    <mergeCell ref="AR8:AX8"/>
+    <mergeCell ref="AY8:BE8"/>
     <mergeCell ref="B2:G4"/>
     <mergeCell ref="I8:O8"/>
     <mergeCell ref="P8:V8"/>
     <mergeCell ref="W8:AC8"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="BF8:BI8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="AD8:AJ8"/>
-    <mergeCell ref="AK8:AQ8"/>
-    <mergeCell ref="AR8:AX8"/>
-    <mergeCell ref="AY8:BE8"/>
+    <mergeCell ref="A22:B22"/>
   </mergeCells>
-  <conditionalFormatting sqref="I11:BI14 I17:BI17 I22:BI24 I26:BI28 I20:BI20 I30:BI44">
-    <cfRule type="expression" dxfId="81" priority="65">
+  <conditionalFormatting sqref="I11:BI12 I18:BI18 I23:BI25 I27:BI29 I21:BI21 I31:BI45 I14:BI14">
+    <cfRule type="expression" dxfId="89" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="67">
+    <cfRule type="expression" dxfId="88" priority="83">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="68">
+    <cfRule type="expression" dxfId="87" priority="84">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="69">
+    <cfRule type="expression" dxfId="86" priority="85">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="70">
+    <cfRule type="expression" dxfId="85" priority="86">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="71">
+    <cfRule type="expression" dxfId="84" priority="87">
       <formula>I$9=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="75">
+    <cfRule type="expression" dxfId="83" priority="91">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="76">
+    <cfRule type="expression" dxfId="82" priority="92">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45:BJ45">
-    <cfRule type="expression" dxfId="73" priority="66">
+  <conditionalFormatting sqref="B46:BJ46">
+    <cfRule type="expression" dxfId="81" priority="82">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:BI9">
-    <cfRule type="expression" dxfId="72" priority="72">
+    <cfRule type="expression" dxfId="80" priority="88">
       <formula>I$9=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BI10">
-    <cfRule type="expression" dxfId="71" priority="57">
+    <cfRule type="expression" dxfId="79" priority="73">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="58">
+    <cfRule type="expression" dxfId="78" priority="74">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="59">
+    <cfRule type="expression" dxfId="77" priority="75">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="60">
+    <cfRule type="expression" dxfId="76" priority="76">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="61">
+    <cfRule type="expression" dxfId="75" priority="77">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="62">
+    <cfRule type="expression" dxfId="74" priority="78">
       <formula>I$9=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="63">
+    <cfRule type="expression" dxfId="73" priority="79">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="64">
+    <cfRule type="expression" dxfId="72" priority="80">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:BI16">
+    <cfRule type="expression" dxfId="71" priority="65">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="66">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="67">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="68">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="69">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="70">
+      <formula>I$9=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="71">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="72">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:BI22">
+    <cfRule type="expression" dxfId="63" priority="57">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="58">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="59">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="60">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="61">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="62">
+      <formula>I$9=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="63">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="64">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26:BI26">
+    <cfRule type="expression" dxfId="55" priority="49">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="50">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="51">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="52">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="53">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="54">
+      <formula>I$9=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="55">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="56">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19:BI19">
+    <cfRule type="expression" dxfId="47" priority="41">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="42">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="43">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="44">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="45">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="46">
+      <formula>I$9=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="47">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="48">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30:BI30">
+    <cfRule type="expression" dxfId="39" priority="33">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="34">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="35">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="36">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>I$9=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="40">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17:BI17">
+    <cfRule type="expression" dxfId="31" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="30">
+      <formula>I$9=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="31">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="32">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20:BI20">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>I$9=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:BI15">
-    <cfRule type="expression" dxfId="63" priority="49">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="50">
+    <cfRule type="expression" dxfId="14" priority="10">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="51">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="53">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>I$9=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="55">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="56">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:BI21">
-    <cfRule type="expression" dxfId="55" priority="41">
+  <conditionalFormatting sqref="I13:BI13">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="42">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="43">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="44">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="45">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="46">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>I$9=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="47">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="48">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25:BI25">
-    <cfRule type="expression" dxfId="47" priority="33">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="34">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="35">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="36">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="37">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="38">
-      <formula>I$9=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="39">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="40">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18:BI18">
-    <cfRule type="expression" dxfId="39" priority="25">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="26">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="27">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="28">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="29">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="30">
-      <formula>I$9=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="31">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="32">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29:BI29">
-    <cfRule type="expression" dxfId="31" priority="17">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="18">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="19">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="20">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="21">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="22">
-      <formula>I$9=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="23">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="24">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16:BI16">
-    <cfRule type="expression" dxfId="23" priority="9">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="10">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="11">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="12">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="13">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
-      <formula>I$9=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="15">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="16">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19:BI19">
-    <cfRule type="expression" dxfId="15" priority="1">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="3">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="4">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
-      <formula>I$9=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update test cases Fix spelling and grammer errors Remove unused activies in gantt chart
</commit_message>
<xml_diff>
--- a/TempestTraceGanttChart.xlsx
+++ b/TempestTraceGanttChart.xlsx
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Plan</t>
   </si>
@@ -117,39 +117,6 @@
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -317,9 +284,6 @@
     <t>End game screen</t>
   </si>
   <si>
-    <t>Game music</t>
-  </si>
-  <si>
     <t>Character sounds</t>
   </si>
   <si>
@@ -327,6 +291,9 @@
   </si>
   <si>
     <t>Level geometry exporter</t>
+  </si>
+  <si>
+    <t>Game music transitions</t>
   </si>
 </sst>
 </file>
@@ -648,7 +615,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -740,9 +707,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
@@ -794,7 +758,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="106">
+  <dxfs count="90">
     <dxf>
       <fill>
         <patternFill>
@@ -1952,232 +1916,6 @@
         </top>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2601,15 +2339,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:BJ45"/>
+  <dimension ref="A2:BJ34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="1" max="1" width="3.625" customWidth="1"/>
     <col min="2" max="2" width="29.25" style="2" customWidth="1"/>
     <col min="3" max="5" width="7.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
@@ -2619,24 +2357,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:62" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="B2" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:62" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
       <c r="I3" s="8" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -2656,11 +2394,11 @@
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="13"/>
       <c r="AD3" s="6" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
@@ -2668,16 +2406,16 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="14"/>
       <c r="AL3" s="6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
@@ -2686,19 +2424,19 @@
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="P5" s="24" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q5" s="22"/>
       <c r="R5" s="20" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="X5" s="21"/>
       <c r="Y5" s="20" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="AE5" s="23"/>
       <c r="AF5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
@@ -2747,13 +2485,13 @@
         <v>7</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
     </row>
     <row r="8" spans="1:62" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
@@ -2763,75 +2501,75 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="36">
+      <c r="I8" s="35">
         <v>42218</v>
       </c>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="37">
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="36">
         <v>42225</v>
       </c>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="37"/>
-      <c r="V8" s="37"/>
-      <c r="W8" s="36">
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="35">
         <v>42232</v>
       </c>
-      <c r="X8" s="36"/>
-      <c r="Y8" s="36"/>
-      <c r="Z8" s="36"/>
-      <c r="AA8" s="36"/>
-      <c r="AB8" s="36"/>
-      <c r="AC8" s="36"/>
-      <c r="AD8" s="37">
+      <c r="X8" s="35"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="35"/>
+      <c r="AA8" s="35"/>
+      <c r="AB8" s="35"/>
+      <c r="AC8" s="35"/>
+      <c r="AD8" s="36">
         <v>42239</v>
       </c>
-      <c r="AE8" s="37"/>
-      <c r="AF8" s="37"/>
-      <c r="AG8" s="37"/>
-      <c r="AH8" s="37"/>
-      <c r="AI8" s="37"/>
-      <c r="AJ8" s="37"/>
-      <c r="AK8" s="36">
+      <c r="AE8" s="36"/>
+      <c r="AF8" s="36"/>
+      <c r="AG8" s="36"/>
+      <c r="AH8" s="36"/>
+      <c r="AI8" s="36"/>
+      <c r="AJ8" s="36"/>
+      <c r="AK8" s="35">
         <v>42246</v>
       </c>
-      <c r="AL8" s="36"/>
-      <c r="AM8" s="36"/>
-      <c r="AN8" s="36"/>
-      <c r="AO8" s="36"/>
-      <c r="AP8" s="36"/>
-      <c r="AQ8" s="36"/>
-      <c r="AR8" s="37">
+      <c r="AL8" s="35"/>
+      <c r="AM8" s="35"/>
+      <c r="AN8" s="35"/>
+      <c r="AO8" s="35"/>
+      <c r="AP8" s="35"/>
+      <c r="AQ8" s="35"/>
+      <c r="AR8" s="36">
         <v>42253</v>
       </c>
-      <c r="AS8" s="37"/>
-      <c r="AT8" s="37"/>
-      <c r="AU8" s="37"/>
-      <c r="AV8" s="37"/>
-      <c r="AW8" s="37"/>
-      <c r="AX8" s="37"/>
-      <c r="AY8" s="36">
+      <c r="AS8" s="36"/>
+      <c r="AT8" s="36"/>
+      <c r="AU8" s="36"/>
+      <c r="AV8" s="36"/>
+      <c r="AW8" s="36"/>
+      <c r="AX8" s="36"/>
+      <c r="AY8" s="35">
         <v>42260</v>
       </c>
-      <c r="AZ8" s="36"/>
-      <c r="BA8" s="36"/>
-      <c r="BB8" s="36"/>
-      <c r="BC8" s="36"/>
-      <c r="BD8" s="36"/>
-      <c r="BE8" s="36"/>
-      <c r="BF8" s="39">
+      <c r="AZ8" s="35"/>
+      <c r="BA8" s="35"/>
+      <c r="BB8" s="35"/>
+      <c r="BC8" s="35"/>
+      <c r="BD8" s="35"/>
+      <c r="BE8" s="35"/>
+      <c r="BF8" s="38">
         <v>42267</v>
       </c>
-      <c r="BG8" s="40"/>
-      <c r="BH8" s="40"/>
-      <c r="BI8" s="40"/>
+      <c r="BG8" s="39"/>
+      <c r="BH8" s="39"/>
+      <c r="BI8" s="39"/>
     </row>
     <row r="9" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -3004,10 +2742,10 @@
       <c r="BJ9" s="1"/>
     </row>
     <row r="10" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="42"/>
+      <c r="A10" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="41"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -3019,7 +2757,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C11" s="15">
         <v>2</v>
@@ -3039,11 +2777,11 @@
       <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33">
+      <c r="A12" s="32">
         <v>2</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C12" s="15">
         <v>4</v>
@@ -3063,11 +2801,11 @@
       <c r="H12" s="27"/>
     </row>
     <row r="13" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33">
+      <c r="A13" s="32">
         <v>3</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C13" s="15">
         <v>14</v>
@@ -3090,11 +2828,11 @@
       </c>
     </row>
     <row r="14" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33">
+      <c r="A14" s="32">
         <v>4</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C14" s="15">
         <v>17</v>
@@ -3111,7 +2849,7 @@
       <c r="G14" s="26">
         <v>0</v>
       </c>
-      <c r="H14" s="34" t="str">
+      <c r="H14" s="33" t="str">
         <f>CONCATENATE(A12, ", ", A29,", ",A13)</f>
         <v>2, 16, 3</v>
       </c>
@@ -3121,7 +2859,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C15" s="15">
         <v>30</v>
@@ -3144,10 +2882,10 @@
       </c>
     </row>
     <row r="16" spans="1:62" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="38"/>
+      <c r="A16" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="37"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -3155,11 +2893,11 @@
       <c r="G16" s="16"/>
     </row>
     <row r="17" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33">
+      <c r="A17" s="32">
         <v>6</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C17" s="15">
         <v>6</v>
@@ -3179,11 +2917,11 @@
       <c r="H17" s="27"/>
     </row>
     <row r="18" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33">
+      <c r="A18" s="32">
         <v>7</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C18" s="15">
         <v>17</v>
@@ -3203,11 +2941,11 @@
       <c r="H18" s="27"/>
     </row>
     <row r="19" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33">
+      <c r="A19" s="32">
         <v>8</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C19" s="15">
         <v>17</v>
@@ -3227,11 +2965,11 @@
       <c r="H19" s="27"/>
     </row>
     <row r="20" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33">
+      <c r="A20" s="32">
         <v>9</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C20" s="15">
         <v>22</v>
@@ -3251,11 +2989,11 @@
       <c r="H20" s="27"/>
     </row>
     <row r="21" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33">
+      <c r="A21" s="32">
         <v>10</v>
       </c>
-      <c r="B21" s="32" t="s">
-        <v>54</v>
+      <c r="B21" s="31" t="s">
+        <v>42</v>
       </c>
       <c r="C21" s="15">
         <v>19</v>
@@ -3275,10 +3013,10 @@
       <c r="H21" s="27"/>
     </row>
     <row r="22" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="38"/>
+      <c r="A22" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="37"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
@@ -3290,8 +3028,8 @@
       <c r="A23" s="29">
         <v>11</v>
       </c>
-      <c r="B23" s="32" t="s">
-        <v>37</v>
+      <c r="B23" s="31" t="s">
+        <v>26</v>
       </c>
       <c r="C23" s="15">
         <v>22</v>
@@ -3315,7 +3053,7 @@
         <v>12</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C24" s="15">
         <v>29</v>
@@ -3341,8 +3079,8 @@
       <c r="A25" s="29">
         <v>13</v>
       </c>
-      <c r="B25" s="32" t="s">
-        <v>32</v>
+      <c r="B25" s="31" t="s">
+        <v>21</v>
       </c>
       <c r="C25" s="15">
         <v>29</v>
@@ -3365,10 +3103,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="38"/>
+      <c r="A26" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="37"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
@@ -3380,8 +3118,8 @@
       <c r="A27" s="29">
         <v>14</v>
       </c>
-      <c r="B27" s="32" t="s">
-        <v>33</v>
+      <c r="B27" s="31" t="s">
+        <v>22</v>
       </c>
       <c r="C27" s="15">
         <v>37</v>
@@ -3405,7 +3143,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C28" s="15">
         <v>40</v>
@@ -3428,8 +3166,8 @@
       <c r="A29" s="29">
         <v>16</v>
       </c>
-      <c r="B29" s="32" t="s">
-        <v>46</v>
+      <c r="B29" s="31" t="s">
+        <v>35</v>
       </c>
       <c r="C29" s="15">
         <v>9</v>
@@ -3452,8 +3190,8 @@
       <c r="A30" s="29">
         <v>17</v>
       </c>
-      <c r="B30" s="32" t="s">
-        <v>49</v>
+      <c r="B30" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="C30" s="17">
         <v>16</v>
@@ -3470,7 +3208,7 @@
       <c r="G30" s="26">
         <v>0</v>
       </c>
-      <c r="H30" s="34">
+      <c r="H30" s="33">
         <f>A12</f>
         <v>2</v>
       </c>
@@ -3479,8 +3217,8 @@
       <c r="A31" s="29">
         <v>18</v>
       </c>
-      <c r="B31" s="32" t="s">
-        <v>50</v>
+      <c r="B31" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="C31" s="17">
         <v>2</v>
@@ -3497,14 +3235,14 @@
       <c r="G31" s="26">
         <v>1</v>
       </c>
-      <c r="H31" s="34"/>
+      <c r="H31" s="33"/>
     </row>
     <row r="32" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>19</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C32" s="15">
         <v>40</v>
@@ -3528,7 +3266,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C33" s="15">
         <v>40</v>
@@ -3551,8 +3289,8 @@
       <c r="A34" s="29">
         <v>21</v>
       </c>
-      <c r="B34" s="32" t="s">
-        <v>52</v>
+      <c r="B34" s="31" t="s">
+        <v>44</v>
       </c>
       <c r="C34" s="15">
         <v>29</v>
@@ -3570,270 +3308,6 @@
         <v>0</v>
       </c>
       <c r="H34" s="27"/>
-    </row>
-    <row r="35" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29">
-        <v>17</v>
-      </c>
-      <c r="B35" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="15">
-        <v>0</v>
-      </c>
-      <c r="D35" s="15">
-        <v>0</v>
-      </c>
-      <c r="E35" s="15">
-        <v>0</v>
-      </c>
-      <c r="F35" s="15">
-        <v>0</v>
-      </c>
-      <c r="G35" s="26">
-        <v>0</v>
-      </c>
-      <c r="H35" s="27"/>
-    </row>
-    <row r="36" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29">
-        <v>18</v>
-      </c>
-      <c r="B36" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="15">
-        <v>0</v>
-      </c>
-      <c r="D36" s="15">
-        <v>0</v>
-      </c>
-      <c r="E36" s="15">
-        <v>0</v>
-      </c>
-      <c r="F36" s="15">
-        <v>0</v>
-      </c>
-      <c r="G36" s="26">
-        <v>0</v>
-      </c>
-      <c r="H36" s="27"/>
-    </row>
-    <row r="37" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="29">
-        <v>19</v>
-      </c>
-      <c r="B37" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="15">
-        <v>0</v>
-      </c>
-      <c r="D37" s="15">
-        <v>0</v>
-      </c>
-      <c r="E37" s="15">
-        <v>0</v>
-      </c>
-      <c r="F37" s="15">
-        <v>0</v>
-      </c>
-      <c r="G37" s="26">
-        <v>0</v>
-      </c>
-      <c r="H37" s="27"/>
-    </row>
-    <row r="38" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29">
-        <v>20</v>
-      </c>
-      <c r="B38" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="15">
-        <v>0</v>
-      </c>
-      <c r="D38" s="15">
-        <v>0</v>
-      </c>
-      <c r="E38" s="15">
-        <v>0</v>
-      </c>
-      <c r="F38" s="15">
-        <v>0</v>
-      </c>
-      <c r="G38" s="26">
-        <v>0</v>
-      </c>
-      <c r="H38" s="27"/>
-    </row>
-    <row r="39" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="29">
-        <v>21</v>
-      </c>
-      <c r="B39" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="15">
-        <v>0</v>
-      </c>
-      <c r="D39" s="15">
-        <v>0</v>
-      </c>
-      <c r="E39" s="15">
-        <v>0</v>
-      </c>
-      <c r="F39" s="15">
-        <v>0</v>
-      </c>
-      <c r="G39" s="26">
-        <v>0</v>
-      </c>
-      <c r="H39" s="27"/>
-    </row>
-    <row r="40" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="29">
-        <v>22</v>
-      </c>
-      <c r="B40" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="15">
-        <v>0</v>
-      </c>
-      <c r="D40" s="15">
-        <v>0</v>
-      </c>
-      <c r="E40" s="15">
-        <v>0</v>
-      </c>
-      <c r="F40" s="15">
-        <v>0</v>
-      </c>
-      <c r="G40" s="26">
-        <v>0</v>
-      </c>
-      <c r="H40" s="27"/>
-    </row>
-    <row r="41" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29">
-        <v>23</v>
-      </c>
-      <c r="B41" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="15">
-        <v>0</v>
-      </c>
-      <c r="D41" s="15">
-        <v>0</v>
-      </c>
-      <c r="E41" s="15">
-        <v>0</v>
-      </c>
-      <c r="F41" s="15">
-        <v>0</v>
-      </c>
-      <c r="G41" s="26">
-        <v>0</v>
-      </c>
-      <c r="H41" s="27"/>
-    </row>
-    <row r="42" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29">
-        <v>24</v>
-      </c>
-      <c r="B42" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="15">
-        <v>0</v>
-      </c>
-      <c r="D42" s="15">
-        <v>0</v>
-      </c>
-      <c r="E42" s="15">
-        <v>0</v>
-      </c>
-      <c r="F42" s="15">
-        <v>0</v>
-      </c>
-      <c r="G42" s="26">
-        <v>0</v>
-      </c>
-      <c r="H42" s="27"/>
-    </row>
-    <row r="43" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="29">
-        <v>25</v>
-      </c>
-      <c r="B43" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="15">
-        <v>0</v>
-      </c>
-      <c r="D43" s="15">
-        <v>0</v>
-      </c>
-      <c r="E43" s="15">
-        <v>0</v>
-      </c>
-      <c r="F43" s="15">
-        <v>0</v>
-      </c>
-      <c r="G43" s="26">
-        <v>0</v>
-      </c>
-      <c r="H43" s="27"/>
-    </row>
-    <row r="44" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="29">
-        <v>26</v>
-      </c>
-      <c r="B44" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="15">
-        <v>0</v>
-      </c>
-      <c r="D44" s="15">
-        <v>0</v>
-      </c>
-      <c r="E44" s="15">
-        <v>0</v>
-      </c>
-      <c r="F44" s="15">
-        <v>0</v>
-      </c>
-      <c r="G44" s="26">
-        <v>0</v>
-      </c>
-      <c r="H44" s="27"/>
-    </row>
-    <row r="45" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="29">
-        <v>27</v>
-      </c>
-      <c r="B45" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" s="15">
-        <v>0</v>
-      </c>
-      <c r="D45" s="15">
-        <v>0</v>
-      </c>
-      <c r="E45" s="15">
-        <v>0</v>
-      </c>
-      <c r="F45" s="15">
-        <v>0</v>
-      </c>
-      <c r="G45" s="26">
-        <v>0</v>
-      </c>
-      <c r="H45" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3852,7 +3326,7 @@
     <mergeCell ref="W8:AC8"/>
     <mergeCell ref="A22:B22"/>
   </mergeCells>
-  <conditionalFormatting sqref="I11:BI12 I18:BI18 I23:BI25 I27:BI29 I21:BI21 I31:BI45 I14:BI14">
+  <conditionalFormatting sqref="I11:BI12 I18:BI18 I23:BI25 I27:BI29 I21:BI21 I31:BI34 I14:BI14">
     <cfRule type="expression" dxfId="89" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3878,7 +3352,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46:BJ46">
+  <conditionalFormatting sqref="B35:BJ35">
     <cfRule type="expression" dxfId="81" priority="82">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add updated Gantt chart Add one missing activity
</commit_message>
<xml_diff>
--- a/TempestTraceGanttChart.xlsx
+++ b/TempestTraceGanttChart.xlsx
@@ -20,6 +20,7 @@
     <definedName name="Plan">PeriodInPlan*(TempestTraceGanttChart!$C1&gt;0)</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -87,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Plan</t>
   </si>
@@ -295,12 +296,36 @@
   <si>
     <t>Game music transitions</t>
   </si>
+  <si>
+    <t>Head-up display</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Dynamic movement</t>
+  </si>
+  <si>
+    <t>Respawn</t>
+  </si>
+  <si>
+    <t>Checkpoints</t>
+  </si>
+  <si>
+    <t>Motion Blur</t>
+  </si>
+  <si>
+    <t>Head bob</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -453,8 +478,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.5"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -532,6 +573,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -615,7 +662,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -741,6 +788,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="14" borderId="3" xfId="3" applyFont="1" applyFill="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2054,7 +2107,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="6"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="20"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2339,10 +2392,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:BJ34"/>
+  <dimension ref="A2:BJ42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2381,7 +2434,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -2637,7 +2690,7 @@
       <c r="AA9" s="3">
         <v>19</v>
       </c>
-      <c r="AB9" s="19">
+      <c r="AB9" s="43">
         <v>20</v>
       </c>
       <c r="AC9" s="3">
@@ -2763,16 +2816,16 @@
         <v>2</v>
       </c>
       <c r="D11" s="15">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E11" s="15">
         <v>2</v>
       </c>
       <c r="F11" s="15">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G11" s="26">
-        <v>0.55000000000000004</v>
+        <v>0.85</v>
       </c>
       <c r="H11" s="27"/>
     </row>
@@ -2787,16 +2840,16 @@
         <v>4</v>
       </c>
       <c r="D12" s="15">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E12" s="15">
         <v>4</v>
       </c>
       <c r="F12" s="15">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G12" s="26">
-        <v>0.25</v>
+        <v>0.7</v>
       </c>
       <c r="H12" s="27"/>
     </row>
@@ -2808,13 +2861,13 @@
         <v>43</v>
       </c>
       <c r="C13" s="15">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D13" s="15">
         <v>3</v>
       </c>
       <c r="E13" s="15">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F13" s="15">
         <v>3</v>
@@ -2835,24 +2888,21 @@
         <v>29</v>
       </c>
       <c r="C14" s="15">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="15">
         <v>13</v>
       </c>
       <c r="E14" s="15">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="15">
         <v>13</v>
       </c>
       <c r="G14" s="26">
-        <v>0</v>
-      </c>
-      <c r="H14" s="33" t="str">
-        <f>CONCATENATE(A12, ", ", A29,", ",A13)</f>
-        <v>2, 16, 3</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="1:62" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
@@ -2912,7 +2962,7 @@
         <v>11</v>
       </c>
       <c r="G17" s="26">
-        <v>0.05</v>
+        <v>0.95</v>
       </c>
       <c r="H17" s="27"/>
     </row>
@@ -2960,7 +3010,7 @@
         <v>12</v>
       </c>
       <c r="G19" s="26">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H19" s="27"/>
     </row>
@@ -2993,55 +3043,67 @@
         <v>10</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C21" s="15">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D21" s="15">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E21" s="15">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F21" s="15">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G21" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="27"/>
     </row>
     <row r="22" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="26"/>
+      <c r="A22" s="32">
+        <v>11</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="15">
+        <v>15</v>
+      </c>
+      <c r="D22" s="15">
+        <v>3</v>
+      </c>
+      <c r="E22" s="15">
+        <v>15</v>
+      </c>
+      <c r="F22" s="15">
+        <v>3</v>
+      </c>
+      <c r="G22" s="26">
+        <v>1</v>
+      </c>
       <c r="H22" s="27"/>
     </row>
     <row r="23" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
-        <v>11</v>
+      <c r="A23" s="32">
+        <v>12</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C23" s="15">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D23" s="15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E23" s="15">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F23" s="15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G23" s="26">
         <v>0</v>
@@ -3049,62 +3111,56 @@
       <c r="H23" s="27"/>
     </row>
     <row r="24" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
-        <v>12</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>20</v>
+      <c r="A24" s="32">
+        <v>13</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="C24" s="15">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D24" s="15">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E24" s="15">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F24" s="15">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G24" s="26">
         <v>0</v>
       </c>
-      <c r="H24" s="27">
-        <f>A23</f>
-        <v>11</v>
-      </c>
+      <c r="H24" s="27"/>
     </row>
     <row r="25" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
-        <v>13</v>
+      <c r="A25" s="32">
+        <v>14</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C25" s="15">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D25" s="15">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E25" s="15">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F25" s="15">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G25" s="26">
         <v>0</v>
       </c>
-      <c r="H25" s="27">
-        <f>A23</f>
-        <v>11</v>
-      </c>
+      <c r="H25" s="27"/>
     </row>
     <row r="26" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="37"/>
       <c r="C26" s="15"/>
@@ -3116,148 +3172,139 @@
     </row>
     <row r="27" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
-        <v>14</v>
-      </c>
-      <c r="B27" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="15">
         <v>22</v>
       </c>
-      <c r="C27" s="15">
-        <v>37</v>
-      </c>
       <c r="D27" s="15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E27" s="15">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F27" s="15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G27" s="26">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H27" s="27"/>
     </row>
     <row r="28" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C28" s="15">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D28" s="15">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E28" s="15">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F28" s="15">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G28" s="26">
         <v>0</v>
       </c>
-      <c r="H28" s="27"/>
+      <c r="H28" s="27">
+        <f>A27</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C29" s="15">
+        <v>29</v>
+      </c>
+      <c r="D29" s="15">
         <v>9</v>
       </c>
-      <c r="D29" s="15">
-        <v>5</v>
-      </c>
       <c r="E29" s="15">
+        <v>29</v>
+      </c>
+      <c r="F29" s="15">
         <v>9</v>
-      </c>
-      <c r="F29" s="15">
-        <v>5</v>
       </c>
       <c r="G29" s="26">
         <v>0</v>
       </c>
-      <c r="H29" s="27"/>
+      <c r="H29" s="27">
+        <f>A27</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
-        <v>17</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="17">
-        <v>16</v>
-      </c>
-      <c r="D30" s="15">
-        <v>3</v>
-      </c>
-      <c r="E30" s="15">
-        <v>16</v>
-      </c>
-      <c r="F30" s="15">
-        <v>3</v>
-      </c>
-      <c r="G30" s="26">
-        <v>0</v>
-      </c>
-      <c r="H30" s="33">
-        <f>A12</f>
-        <v>2</v>
-      </c>
+      <c r="A30" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="27"/>
     </row>
     <row r="31" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>18</v>
       </c>
-      <c r="B31" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="17">
-        <v>2</v>
+      <c r="B31" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="15">
+        <v>17</v>
       </c>
       <c r="D31" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" s="15">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F31" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31" s="26">
         <v>1</v>
       </c>
-      <c r="H31" s="33"/>
+      <c r="H31" s="27"/>
     </row>
     <row r="32" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>19</v>
       </c>
-      <c r="B32" s="28" t="s">
-        <v>37</v>
+      <c r="B32" s="42" t="s">
+        <v>47</v>
       </c>
       <c r="C32" s="15">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D32" s="15">
         <v>10</v>
       </c>
       <c r="E32" s="15">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="F32" s="15">
         <v>10</v>
       </c>
       <c r="G32" s="26">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H32" s="27"/>
     </row>
@@ -3265,53 +3312,236 @@
       <c r="A33" s="29">
         <v>20</v>
       </c>
-      <c r="B33" s="30" t="s">
-        <v>40</v>
+      <c r="B33" s="42" t="s">
+        <v>46</v>
       </c>
       <c r="C33" s="15">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D33" s="15">
         <v>3</v>
       </c>
       <c r="E33" s="15">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="F33" s="15">
         <v>3</v>
       </c>
       <c r="G33" s="26">
+        <v>1</v>
+      </c>
+      <c r="H33" s="27"/>
+    </row>
+    <row r="34" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="37"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="27"/>
+    </row>
+    <row r="35" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="29">
+        <v>21</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="15">
+        <v>37</v>
+      </c>
+      <c r="D35" s="15">
+        <v>5</v>
+      </c>
+      <c r="E35" s="15">
+        <v>37</v>
+      </c>
+      <c r="F35" s="15">
+        <v>5</v>
+      </c>
+      <c r="G35" s="26">
         <v>0</v>
       </c>
-      <c r="H33" s="27"/>
-    </row>
-    <row r="34" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="29">
-        <v>21</v>
-      </c>
-      <c r="B34" s="31" t="s">
+      <c r="H35" s="27"/>
+    </row>
+    <row r="36" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29">
+        <v>22</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="15">
+        <v>40</v>
+      </c>
+      <c r="D36" s="15">
+        <v>5</v>
+      </c>
+      <c r="E36" s="15">
+        <v>40</v>
+      </c>
+      <c r="F36" s="15">
+        <v>5</v>
+      </c>
+      <c r="G36" s="26">
+        <v>0</v>
+      </c>
+      <c r="H36" s="27"/>
+    </row>
+    <row r="37" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="29">
+        <v>23</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="15">
+        <v>9</v>
+      </c>
+      <c r="D37" s="15">
+        <v>5</v>
+      </c>
+      <c r="E37" s="15">
+        <v>9</v>
+      </c>
+      <c r="F37" s="15">
+        <v>5</v>
+      </c>
+      <c r="G37" s="26">
+        <v>1</v>
+      </c>
+      <c r="H37" s="27"/>
+    </row>
+    <row r="38" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="29">
+        <v>24</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="17">
+        <v>25</v>
+      </c>
+      <c r="D38" s="15">
+        <v>3</v>
+      </c>
+      <c r="E38" s="15">
+        <v>25</v>
+      </c>
+      <c r="F38" s="15">
+        <v>3</v>
+      </c>
+      <c r="G38" s="26">
+        <v>0</v>
+      </c>
+      <c r="H38" s="33">
+        <f>A12</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="29">
+        <v>25</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="17">
+        <v>2</v>
+      </c>
+      <c r="D39" s="15">
+        <v>2</v>
+      </c>
+      <c r="E39" s="15">
+        <v>2</v>
+      </c>
+      <c r="F39" s="15">
+        <v>2</v>
+      </c>
+      <c r="G39" s="26">
+        <v>1</v>
+      </c>
+      <c r="H39" s="33"/>
+    </row>
+    <row r="40" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="29">
+        <v>26</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="15">
+        <v>40</v>
+      </c>
+      <c r="D40" s="15">
+        <v>10</v>
+      </c>
+      <c r="E40" s="15">
+        <v>40</v>
+      </c>
+      <c r="F40" s="15">
+        <v>10</v>
+      </c>
+      <c r="G40" s="26">
+        <v>0</v>
+      </c>
+      <c r="H40" s="27"/>
+    </row>
+    <row r="41" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="29">
+        <v>27</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="15">
+        <v>40</v>
+      </c>
+      <c r="D41" s="15">
+        <v>3</v>
+      </c>
+      <c r="E41" s="15">
+        <v>40</v>
+      </c>
+      <c r="F41" s="15">
+        <v>3</v>
+      </c>
+      <c r="G41" s="26">
+        <v>0</v>
+      </c>
+      <c r="H41" s="27"/>
+    </row>
+    <row r="42" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="29">
+        <v>28</v>
+      </c>
+      <c r="B42" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C42" s="15">
         <v>29</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D42" s="15">
         <v>2</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E42" s="15">
         <v>29</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F42" s="15">
         <v>2</v>
       </c>
-      <c r="G34" s="26">
+      <c r="G42" s="26">
         <v>0</v>
       </c>
-      <c r="H34" s="27"/>
+      <c r="H42" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A26:B26"/>
+  <mergeCells count="15">
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="BF8:BI8"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="A10:B10"/>
@@ -3320,13 +3550,14 @@
     <mergeCell ref="AK8:AQ8"/>
     <mergeCell ref="AR8:AX8"/>
     <mergeCell ref="AY8:BE8"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="B2:G4"/>
     <mergeCell ref="I8:O8"/>
     <mergeCell ref="P8:V8"/>
     <mergeCell ref="W8:AC8"/>
-    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
-  <conditionalFormatting sqref="I11:BI12 I18:BI18 I23:BI25 I27:BI29 I21:BI21 I31:BI34 I14:BI14">
+  <conditionalFormatting sqref="I11:BI12 I18:BI18 I27:BI33 I35:BI37 I25:BI25 I39:BI42 I14:BI14">
     <cfRule type="expression" dxfId="89" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3352,7 +3583,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:BJ35">
+  <conditionalFormatting sqref="B43:BJ43">
     <cfRule type="expression" dxfId="81" priority="82">
       <formula>TRUE</formula>
     </cfRule>
@@ -3414,7 +3645,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22:BI22">
+  <conditionalFormatting sqref="I26:BI26">
     <cfRule type="expression" dxfId="63" priority="57">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3440,7 +3671,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26:BI26">
+  <conditionalFormatting sqref="I34:BI34">
     <cfRule type="expression" dxfId="55" priority="49">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3492,7 +3723,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30:BI30">
+  <conditionalFormatting sqref="I38:BI38">
     <cfRule type="expression" dxfId="39" priority="33">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3544,7 +3775,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:BI20">
+  <conditionalFormatting sqref="I20:BI24">
     <cfRule type="expression" dxfId="23" priority="17">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>